<commit_message>
Settings changed in controller sheet
</commit_message>
<xml_diff>
--- a/src/test/java/com/SL8Z/xls/Controller.xlsx
+++ b/src/test/java/com/SL8Z/xls/Controller.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2508" windowWidth="13968" windowHeight="5052" tabRatio="320"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13965" windowHeight="5055" tabRatio="320"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -125,8 +125,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -284,6 +284,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -318,6 +319,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,22 +495,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="86.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125"/>
-    <col min="4" max="1025" width="8.6640625"/>
+    <col min="2" max="2" width="86.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625"/>
+    <col min="4" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" customHeight="1">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -519,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -530,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -552,7 +554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -563,7 +565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -574,7 +576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -585,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -596,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -607,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -618,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -629,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -640,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -648,10 +650,10 @@
         <v>32</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>31</v>
       </c>
@@ -662,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -670,7 +672,7 @@
         <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -680,29 +682,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>